<commit_message>
made pca plots, updated some excel stuff
</commit_message>
<xml_diff>
--- a/data/01_pd-samples/26_02-10_SraRunTable.xlsx
+++ b/data/01_pd-samples/26_02-10_SraRunTable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caprinapugliese/Documents/School/Uconn/2024-26_Grad_School/Dagilis-lab/WNS-project/data/01_pd-samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{1C46A98D-EEFD-4641-AEB8-E287520693CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B09D600-2B26-FE49-8FDE-6F0D03C97207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="27360" windowHeight="16940" activeTab="1" xr2:uid="{EE856442-0BA1-BF46-A55B-3F040DC28406}"/>
   </bookViews>
@@ -3298,7 +3298,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3478,6 +3478,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -3639,9 +3645,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3687,7 +3694,11 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yy"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -3698,6 +3709,96 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A43B09ED-D87A-2E4D-82D8-DB35E4ED55D2}" name="Table1" displayName="Table1" ref="A1:BF131" totalsRowShown="0">
+  <autoFilter ref="A1:BF131" xr:uid="{A43B09ED-D87A-2E4D-82D8-DB35E4ED55D2}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Illumina Genome Analyzer IIx"/>
+        <filter val="Illumina HiSeq 2000"/>
+        <filter val="Illumina MiSeq"/>
+        <filter val="Illumina NovaSeq 6000"/>
+        <filter val="Ion Torrent PGM"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="7">
+      <filters>
+        <filter val="ILLUMINA"/>
+        <filter val="ION_TORRENT"/>
+        <filter val="LS454"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="14">
+      <filters blank="1">
+        <filter val="Canada"/>
+        <filter val="USA"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <tableColumns count="58">
+    <tableColumn id="1" xr3:uid="{82D4CCBE-B150-B54C-97AC-099C753FB20B}" name="Run"/>
+    <tableColumn id="2" xr3:uid="{3AC929BB-D94A-6B47-8A66-DF774EAABC32}" name="Collection_Date" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{A68E7A4C-73D3-434E-A3C1-B629BF8EC557}" name="Instrument"/>
+    <tableColumn id="4" xr3:uid="{D1582B5F-59C5-4E4F-8D57-C009B796DB0F}" name="LibraryLayout"/>
+    <tableColumn id="5" xr3:uid="{3BB26B96-A1F2-854A-89EE-E671DA006712}" name="LibrarySelection"/>
+    <tableColumn id="6" xr3:uid="{70CF03E0-9B8C-D14D-9372-D5B452BE785B}" name="LibrarySource"/>
+    <tableColumn id="7" xr3:uid="{F04B4F76-2408-A84B-8AFD-D89B340432FB}" name="Organism"/>
+    <tableColumn id="8" xr3:uid="{0D0784A4-AE18-4D40-A4B7-D4BED26BE9E6}" name="Platform"/>
+    <tableColumn id="9" xr3:uid="{BC249215-C0C3-614D-817C-3BD1A9DE57BE}" name="ReleaseDate"/>
+    <tableColumn id="10" xr3:uid="{826B512F-0516-2947-99A0-A15C629FA24A}" name="create_date"/>
+    <tableColumn id="11" xr3:uid="{2EF1739F-0B52-E54C-B472-F0A3CE7A35BE}" name="version"/>
+    <tableColumn id="12" xr3:uid="{86D3DBCF-9DC9-3448-86A1-0BE520385007}" name="Sample Name"/>
+    <tableColumn id="13" xr3:uid="{76AE9B38-BA87-7647-BF34-E63550C42A85}" name="SRA Study"/>
+    <tableColumn id="14" xr3:uid="{11D8FF47-674E-7D44-84D2-5C7271E4668B}" name="BioSampleModel"/>
+    <tableColumn id="15" xr3:uid="{E38D9F5A-235A-C14A-A2F6-3DCA6E27ED4B}" name="geo_loc_name_country"/>
+    <tableColumn id="16" xr3:uid="{8B1C8950-E696-0949-BF3C-8B7F344C301B}" name="geo_loc_name_country_continent"/>
+    <tableColumn id="17" xr3:uid="{A63F81AC-A1FC-3747-9019-E793474A6271}" name="geo_loc_name"/>
+    <tableColumn id="18" xr3:uid="{D58C98E1-7351-9B46-AB6F-B0E1CC7D25EC}" name="HOST"/>
+    <tableColumn id="19" xr3:uid="{E8AF0C36-C7EC-DA43-A716-81D4BA1FD948}" name="strain"/>
+    <tableColumn id="20" xr3:uid="{7F81AEEB-FD09-F743-A0E7-D6A9502D86FD}" name="lat_lon"/>
+    <tableColumn id="21" xr3:uid="{E2294093-81FE-1C49-B98A-A97BB90EA23C}" name="sample_type"/>
+    <tableColumn id="22" xr3:uid="{90779EA3-33BE-B44C-8834-75540C84E1C2}" name="isolation_source"/>
+    <tableColumn id="23" xr3:uid="{34BAA073-958A-F14B-B84E-A90C6F0A691A}" name="isolate"/>
+    <tableColumn id="24" xr3:uid="{6AD30FFB-043D-894C-AB55-729225B4828A}" name="mating_type"/>
+    <tableColumn id="25" xr3:uid="{4675FFCB-9593-094E-91C9-CFD4F45D8773}" name="host_tissue_sampled"/>
+    <tableColumn id="26" xr3:uid="{98CEBE0E-2259-D246-A20E-D5B6C272063B}" name="BIOMATERIAL_PROVIDER"/>
+    <tableColumn id="27" xr3:uid="{9B918539-BFEE-AA40-92FE-D3C777B7035F}" name="env_broad_scale"/>
+    <tableColumn id="28" xr3:uid="{FE28C878-E5F7-5249-8F22-A321D385D4A6}" name="Cultivar"/>
+    <tableColumn id="29" xr3:uid="{DCED73D8-B9DD-E146-ACCF-988EFCDCAFF1}" name="ecotype"/>
+    <tableColumn id="30" xr3:uid="{A4FD608C-2C42-8C4C-8AD9-85C9AD005C18}" name="env_local_scale"/>
+    <tableColumn id="31" xr3:uid="{E175B873-862B-7843-809F-C9EAA26DA2CC}" name="env_medium"/>
+    <tableColumn id="32" xr3:uid="{740D9BA2-28DA-944E-84F2-DD39CD38E610}" name="isol_growth_condt"/>
+    <tableColumn id="33" xr3:uid="{B0988164-3F08-CC42-9726-4715AF1AEDDD}" name="collected_by"/>
+    <tableColumn id="34" xr3:uid="{68463C8F-EB0C-064C-A737-DD07FC472FF5}" name="isolate_name_alias"/>
+    <tableColumn id="35" xr3:uid="{876A7CC7-560B-9942-B641-623F71DDCE08}" name="Host_disease"/>
+    <tableColumn id="36" xr3:uid="{193260B7-93EC-3B47-AA7D-3CB3F1EF84D3}" name="analysis_type (exp)"/>
+    <tableColumn id="37" xr3:uid="{E8931442-5BD4-354B-8312-C669517F0520}" name="analysis_type (run)"/>
+    <tableColumn id="38" xr3:uid="{4AEAE4BF-721A-9844-B95C-2077F3700189}" name="geographic_location_(country_and/or_sea"/>
+    <tableColumn id="39" xr3:uid="{CC01C85F-F534-DC46-89BC-A5A44FBD216F}" name="region)"/>
+    <tableColumn id="40" xr3:uid="{169D4EC3-E86D-9A46-9198-BE9F7DE84925}" name="gssr_id (exp)"/>
+    <tableColumn id="41" xr3:uid="{E60B0091-3DD7-5B41-ABA1-9C2714BEE0FA}" name="gssr_id (run)"/>
+    <tableColumn id="42" xr3:uid="{C2C16CDF-0100-AC4A-892E-1ACEB55B08D0}" name="instrument_name (run)"/>
+    <tableColumn id="43" xr3:uid="{18B4ED11-6392-5D4D-A439-5A6C48AF1BDE}" name="lsid (exp)"/>
+    <tableColumn id="44" xr3:uid="{17862725-4C6B-6B45-BA92-53095820FBED}" name="lsid (run)"/>
+    <tableColumn id="45" xr3:uid="{3D46143B-1AD9-C442-A68B-38D7546C3B48}" name="material_type (exp)"/>
+    <tableColumn id="46" xr3:uid="{D1F60095-ADC9-EF4E-9475-DB3E6BF9F32D}" name="molecular_indexing_scheme (run)"/>
+    <tableColumn id="47" xr3:uid="{D1068B64-975B-3B4B-B675-9182834DEACE}" name="project (exp)"/>
+    <tableColumn id="48" xr3:uid="{C7793598-8CDE-844E-A77B-D20B3B50CF91}" name="project (run)"/>
+    <tableColumn id="49" xr3:uid="{7D1847DF-BCC1-6146-ADC5-DF3755DC879E}" name="region (run)"/>
+    <tableColumn id="50" xr3:uid="{A922E147-E569-734F-A6C3-BE25BD5A3A66}" name="run_barcode (run)"/>
+    <tableColumn id="51" xr3:uid="{10416BA6-4BEE-E04E-AB2B-9412716227D8}" name="run_name (run)"/>
+    <tableColumn id="52" xr3:uid="{1265BE24-178A-3945-9F04-31188CD62290}" name="Sample_name"/>
+    <tableColumn id="53" xr3:uid="{CC3AA12E-4B08-0F43-8C0F-E095BF0A731B}" name="specific_host"/>
+    <tableColumn id="54" xr3:uid="{94F17867-B4E3-824E-8328-B2AC307A5FB5}" name="work_request (exp)"/>
+    <tableColumn id="55" xr3:uid="{F294DF9E-5328-E544-A9CA-B9270EA98C13}" name="work_request (run)"/>
+    <tableColumn id="56" xr3:uid="{4AAFD458-8719-8B4F-9265-259A460C76D2}" name="type-material"/>
+    <tableColumn id="57" xr3:uid="{E392710A-ED82-C246-BFF0-A6685B9AA839}" name="Citation"/>
+    <tableColumn id="58" xr3:uid="{3A949A24-A861-024B-8B8B-2795DDEB54CE}" name="identified_by"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -19250,24 +19351,60 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{218F34BE-B9C4-D545-9EA2-9D654AEF65D9}">
   <dimension ref="A1:BG131"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="C99" sqref="C99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.1640625" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
     <col min="7" max="7" width="32.33203125" customWidth="1"/>
     <col min="9" max="9" width="20.5" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
-    <col min="12" max="12" width="31.5" customWidth="1"/>
-    <col min="15" max="15" width="18.1640625" customWidth="1"/>
-    <col min="16" max="16" width="17.6640625" customWidth="1"/>
+    <col min="12" max="12" width="45.5" customWidth="1"/>
+    <col min="13" max="13" width="11.5" customWidth="1"/>
+    <col min="14" max="14" width="62.6640625" customWidth="1"/>
+    <col min="15" max="15" width="22" customWidth="1"/>
+    <col min="16" max="16" width="30.6640625" customWidth="1"/>
     <col min="17" max="17" width="27.5" customWidth="1"/>
-    <col min="18" max="18" width="21.1640625" customWidth="1"/>
+    <col min="18" max="18" width="33" customWidth="1"/>
     <col min="20" max="20" width="27.83203125" customWidth="1"/>
+    <col min="21" max="21" width="15.1640625" customWidth="1"/>
+    <col min="22" max="22" width="34.1640625" customWidth="1"/>
+    <col min="24" max="24" width="13.33203125" customWidth="1"/>
+    <col min="25" max="25" width="20.33203125" customWidth="1"/>
+    <col min="26" max="26" width="25.33203125" customWidth="1"/>
+    <col min="27" max="27" width="17" customWidth="1"/>
+    <col min="30" max="30" width="16.33203125" customWidth="1"/>
+    <col min="31" max="31" width="13.6640625" customWidth="1"/>
+    <col min="32" max="32" width="18.1640625" customWidth="1"/>
+    <col min="33" max="33" width="13.83203125" customWidth="1"/>
+    <col min="34" max="34" width="19" customWidth="1"/>
+    <col min="35" max="35" width="14.33203125" customWidth="1"/>
+    <col min="36" max="36" width="18.83203125" customWidth="1"/>
+    <col min="37" max="37" width="18.6640625" customWidth="1"/>
+    <col min="38" max="38" width="37.33203125" customWidth="1"/>
+    <col min="40" max="40" width="13.5" customWidth="1"/>
+    <col min="41" max="41" width="13.33203125" customWidth="1"/>
+    <col min="42" max="42" width="22" customWidth="1"/>
+    <col min="45" max="45" width="19.1640625" customWidth="1"/>
+    <col min="46" max="46" width="30.6640625" customWidth="1"/>
+    <col min="47" max="47" width="13.83203125" customWidth="1"/>
+    <col min="48" max="48" width="13.6640625" customWidth="1"/>
+    <col min="49" max="49" width="12.83203125" customWidth="1"/>
+    <col min="50" max="50" width="18" customWidth="1"/>
+    <col min="51" max="51" width="15.83203125" customWidth="1"/>
+    <col min="52" max="52" width="14.83203125" customWidth="1"/>
+    <col min="53" max="53" width="14.1640625" customWidth="1"/>
+    <col min="54" max="54" width="18.83203125" customWidth="1"/>
+    <col min="55" max="55" width="18.6640625" customWidth="1"/>
+    <col min="56" max="56" width="14.5" customWidth="1"/>
+    <col min="58" max="58" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:59" x14ac:dyDescent="0.2">
@@ -19449,7 +19586,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:59" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -19514,7 +19651,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:59" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>100</v>
       </c>
@@ -19579,7 +19716,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:59" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>112</v>
       </c>
@@ -19641,7 +19778,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:59" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>121</v>
       </c>
@@ -19703,7 +19840,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:59" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>129</v>
       </c>
@@ -19768,7 +19905,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:59" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>137</v>
       </c>
@@ -19830,7 +19967,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:59" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>148</v>
       </c>
@@ -19892,7 +20029,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:59" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>152</v>
       </c>
@@ -19975,7 +20112,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:59" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>173</v>
       </c>
@@ -20058,7 +20195,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="11" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:59" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>187</v>
       </c>
@@ -20141,7 +20278,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="12" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:59" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>197</v>
       </c>
@@ -20224,7 +20361,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="13" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:59" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>208</v>
       </c>
@@ -20307,7 +20444,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="14" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:59" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>218</v>
       </c>
@@ -20390,7 +20527,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="15" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:59" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>228</v>
       </c>
@@ -20473,7 +20610,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="16" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:59" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>240</v>
       </c>
@@ -20556,7 +20693,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>250</v>
       </c>
@@ -20639,7 +20776,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>261</v>
       </c>
@@ -20722,7 +20859,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>271</v>
       </c>
@@ -20805,7 +20942,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>275</v>
       </c>
@@ -20888,7 +21025,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>279</v>
       </c>
@@ -20971,7 +21108,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>283</v>
       </c>
@@ -21054,7 +21191,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>287</v>
       </c>
@@ -21137,7 +21274,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>291</v>
       </c>
@@ -21220,7 +21357,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>296</v>
       </c>
@@ -21303,7 +21440,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>305</v>
       </c>
@@ -21386,7 +21523,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>313</v>
       </c>
@@ -21469,7 +21606,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>316</v>
       </c>
@@ -21552,7 +21689,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>321</v>
       </c>
@@ -21635,7 +21772,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>324</v>
       </c>
@@ -21718,7 +21855,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>329</v>
       </c>
@@ -21801,7 +21938,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>334</v>
       </c>
@@ -21884,7 +22021,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="33" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>339</v>
       </c>
@@ -21967,7 +22104,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="34" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>345</v>
       </c>
@@ -22050,7 +22187,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="35" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>350</v>
       </c>
@@ -22133,7 +22270,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="36" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>355</v>
       </c>
@@ -22216,7 +22353,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="37" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>361</v>
       </c>
@@ -22299,7 +22436,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="38" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>365</v>
       </c>
@@ -22406,7 +22543,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="39" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>390</v>
       </c>
@@ -22513,7 +22650,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="40" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>394</v>
       </c>
@@ -22620,7 +22757,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="41" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>396</v>
       </c>
@@ -22727,7 +22864,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="42" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>405</v>
       </c>
@@ -22831,7 +22968,7 @@
         <v>21045</v>
       </c>
     </row>
-    <row r="43" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>415</v>
       </c>
@@ -22935,7 +23072,7 @@
         <v>21045</v>
       </c>
     </row>
-    <row r="44" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>421</v>
       </c>
@@ -23039,7 +23176,7 @@
         <v>21045</v>
       </c>
     </row>
-    <row r="45" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>423</v>
       </c>
@@ -23143,7 +23280,7 @@
         <v>21045</v>
       </c>
     </row>
-    <row r="46" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>426</v>
       </c>
@@ -23250,7 +23387,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="47" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>428</v>
       </c>
@@ -23357,7 +23494,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="48" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>429</v>
       </c>
@@ -23727,7 +23864,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="53" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>465</v>
       </c>
@@ -23789,7 +23926,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="54" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>478</v>
       </c>
@@ -23851,7 +23988,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="55" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>484</v>
       </c>
@@ -23913,7 +24050,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="56" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>490</v>
       </c>
@@ -23975,7 +24112,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="57" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>496</v>
       </c>
@@ -24037,7 +24174,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="58" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>502</v>
       </c>
@@ -24099,7 +24236,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="59" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>508</v>
       </c>
@@ -24161,7 +24298,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="60" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>514</v>
       </c>
@@ -24223,7 +24360,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="61" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>520</v>
       </c>
@@ -24285,7 +24422,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="62" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>526</v>
       </c>
@@ -24347,7 +24484,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="63" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>532</v>
       </c>
@@ -24409,7 +24546,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="64" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>537</v>
       </c>
@@ -24471,7 +24608,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="65" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>543</v>
       </c>
@@ -24533,7 +24670,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="66" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>549</v>
       </c>
@@ -24595,7 +24732,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="67" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>555</v>
       </c>
@@ -24657,7 +24794,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="68" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>561</v>
       </c>
@@ -24719,7 +24856,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="69" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>568</v>
       </c>
@@ -24781,7 +24918,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="70" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>573</v>
       </c>
@@ -24843,7 +24980,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="71" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>580</v>
       </c>
@@ -24911,7 +25048,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="72" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>590</v>
       </c>
@@ -24979,7 +25116,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="73" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>597</v>
       </c>
@@ -25047,7 +25184,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="74" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>604</v>
       </c>
@@ -25115,7 +25252,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="75" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>610</v>
       </c>
@@ -25272,7 +25409,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="77" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>636</v>
       </c>
@@ -25349,7 +25486,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="78" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>643</v>
       </c>
@@ -26658,7 +26795,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>756</v>
       </c>
@@ -26735,7 +26872,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>767</v>
       </c>
@@ -26812,7 +26949,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="97" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>775</v>
       </c>
@@ -27496,7 +27633,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="106" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>833</v>
       </c>
@@ -27573,7 +27710,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="107" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>840</v>
       </c>
@@ -27845,68 +27982,68 @@
         <v>464</v>
       </c>
     </row>
-    <row r="111" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
+    <row r="111" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="2" t="s">
         <v>867</v>
       </c>
-      <c r="B111">
+      <c r="B111" s="2">
         <v>2016</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C111" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="D111" t="s">
+      <c r="D111" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="E111" t="s">
+      <c r="E111" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="F111" t="s">
+      <c r="F111" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="G111" t="s">
+      <c r="G111" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="H111" t="s">
+      <c r="H111" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="I111" t="s">
+      <c r="I111" s="2" t="s">
         <v>852</v>
       </c>
-      <c r="J111" t="s">
+      <c r="J111" s="2" t="s">
         <v>853</v>
       </c>
-      <c r="K111">
+      <c r="K111" s="2">
         <v>1</v>
       </c>
-      <c r="L111" t="s">
+      <c r="L111" s="2" t="s">
         <v>870</v>
       </c>
-      <c r="M111" t="s">
+      <c r="M111" s="2" t="s">
         <v>854</v>
       </c>
-      <c r="N111" t="s">
+      <c r="N111" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="O111" t="s">
+      <c r="O111" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="P111" t="s">
+      <c r="P111" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="Q111" t="s">
+      <c r="Q111" s="2" t="s">
         <v>871</v>
       </c>
-      <c r="R111" t="s">
+      <c r="R111" s="2" t="s">
         <v>872</v>
       </c>
-      <c r="S111" t="s">
+      <c r="S111" s="2" t="s">
         <v>870</v>
       </c>
-      <c r="U111" t="s">
+      <c r="U111" s="2" t="s">
         <v>856</v>
       </c>
-      <c r="X111" t="s">
+      <c r="X111" s="2" t="s">
         <v>464</v>
       </c>
     </row>
@@ -29233,7 +29370,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="130" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:58" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>1020</v>
       </c>
@@ -29313,7 +29450,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="131" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:58" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>1040</v>
       </c>
@@ -29392,5 +29529,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>